<commit_message>
Component List updated v2
</commit_message>
<xml_diff>
--- a/Component List/Component List.xlsx
+++ b/Component List/Component List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\EE463-Term-Project-Group-1\Component List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5D1E1B-C818-4BAC-9A09-942F67F17E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B15F08-C8E8-4640-AE93-E921779E37A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2070" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Component</t>
   </si>
@@ -85,6 +85,48 @@
   </si>
   <si>
     <t>x3</t>
+  </si>
+  <si>
+    <t>11,73TL</t>
+  </si>
+  <si>
+    <t>4,69TL</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/pasif-komponentler/kondansatorler/film-kondansatorler/C322J104J60A605</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/pasif-komponentler/direncler/tas-direncler/PRW05WJW10KB00</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/pasif-komponentler/kondansatorler/aluminyum-kondansatorler/PKL5-400V221MN400</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/35a-1000v-kopru-diyot</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/ixgh24n60c4d1-rohs-24a600v-to247ad-igbtdiode</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/tl494--025a-switching-controller-300khz-switching-freq-max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48,35TL </t>
+  </si>
+  <si>
+    <t>36,45TL</t>
+  </si>
+  <si>
+    <t>25TL</t>
+  </si>
+  <si>
+    <t>2,4TL</t>
+  </si>
+  <si>
+    <t>14,65TL</t>
   </si>
 </sst>
 </file>
@@ -413,27 +455,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="128.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -443,8 +489,14 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -454,8 +506,14 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -465,8 +523,14 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -476,8 +540,14 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -487,8 +557,14 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -498,8 +574,14 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -509,17 +591,18 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{0CC0F60C-2343-4D25-867F-C8C293A44A7D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Heat Sink is added to the Component List v3
</commit_message>
<xml_diff>
--- a/Component List/Component List.xlsx
+++ b/Component List/Component List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\EE463-Term-Project-Group-1\Component List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B15F08-C8E8-4640-AE93-E921779E37A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A1C3CB-6B79-419A-AB41-487058B8745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2070" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Component</t>
   </si>
@@ -127,6 +127,42 @@
   </si>
   <si>
     <t>14,65TL</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Current Rating</t>
+  </si>
+  <si>
+    <t>Voltage Rating</t>
+  </si>
+  <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>1000V</t>
+  </si>
+  <si>
+    <t>30A</t>
+  </si>
+  <si>
+    <t>600V</t>
+  </si>
+  <si>
+    <t>400V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Sink </t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/elektromekanik-komponentler/sogutucular/aluminyum-sogutucular/530802B05100G</t>
+  </si>
+  <si>
+    <t>530802B05100G</t>
+  </si>
+  <si>
+    <t>31,6TL</t>
   </si>
 </sst>
 </file>
@@ -455,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,9 +502,11 @@
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="6" max="6" width="128.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +516,14 @@
       <c r="F1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -495,8 +539,17 @@
       <c r="F2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -512,8 +565,17 @@
       <c r="F3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -529,8 +591,17 @@
       <c r="F4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,8 +617,14 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -564,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -581,7 +658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -596,6 +673,23 @@
       </c>
       <c r="F8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>